<commit_message>
Excel to Dict Code
</commit_message>
<xml_diff>
--- a/python/Excel_Python/excel_files/Invoices_App.xlsx
+++ b/python/Excel_Python/excel_files/Invoices_App.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\cohort4\python\Excel_Python\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7418A3A-F75C-457A-9220-44C22E215A8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E6B8BE-EEA3-4DE5-B4CC-2D5587C65B41}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9975" yWindow="-15720" windowWidth="13500" windowHeight="14355" activeTab="3" xr2:uid="{5807CD10-EE00-41D4-B8D5-7B5FFEA8A2BD}"/>
+    <workbookView xWindow="15105" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{5807CD10-EE00-41D4-B8D5-7B5FFEA8A2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="5" r:id="rId1"/>
     <sheet name="Invoices" sheetId="2" r:id="rId2"/>
-    <sheet name="Invoice_list" sheetId="3" r:id="rId3"/>
+    <sheet name="Invoice_list" sheetId="7" r:id="rId3"/>
     <sheet name="products" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -877,10 +877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1151AD-ABE3-4EBD-A751-04C74E7A7844}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1044,9 +1044,6 @@
       <c r="D11" s="3">
         <v>43970</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1055,22 +1052,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E146731-EF1A-46F1-9120-5529797485F7}">
-  <dimension ref="A1:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B437FD4-45FB-4136-B215-D0DB7049F7C6}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1084,7 +1075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1098,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1112,7 +1103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1126,7 +1117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1140,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1154,7 +1145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1168,7 +1159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1182,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1196,7 +1187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1210,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1224,43 +1215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="2"/>
-    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="F13:F22" xr:uid="{8F6F745D-ABD9-424D-9291-67D8C00DBD24}">
-      <formula1>100</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1269,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214CC247-E970-4F1E-BDCF-F7B89A4393EA}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refactored Tax Calc -array, flask api with spa
</commit_message>
<xml_diff>
--- a/python/Excel_Python/excel_files/Invoices_App.xlsx
+++ b/python/Excel_Python/excel_files/Invoices_App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\cohort4\python\Excel_Python\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E6B8BE-EEA3-4DE5-B4CC-2D5587C65B41}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31206310-007D-48F5-A7BD-C41F8CADC294}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15105" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{5807CD10-EE00-41D4-B8D5-7B5FFEA8A2BD}"/>
+    <workbookView xWindow="17940" yWindow="-14940" windowWidth="20595" windowHeight="12855" activeTab="1" xr2:uid="{5807CD10-EE00-41D4-B8D5-7B5FFEA8A2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
   <si>
     <t>customer_id</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>meryl.streep@ymail.com</t>
+  </si>
+  <si>
+    <t>000-2254</t>
+  </si>
+  <si>
+    <t>000-3561</t>
   </si>
 </sst>
 </file>
@@ -877,10 +883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1151AD-ABE3-4EBD-A751-04C74E7A7844}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,6 +1051,34 @@
         <v>43970</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>106</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="3">
+        <v>43972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>102</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43974</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1053,13 +1087,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B437FD4-45FB-4136-B215-D0DB7049F7C6}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1094,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>13</v>
@@ -1213,6 +1253,34 @@
       </c>
       <c r="D11">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1293,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>